<commit_message>
Build raw incidence table
</commit_message>
<xml_diff>
--- a/data/processed/incidence.xlsx
+++ b/data/processed/incidence.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="212">
   <si>
     <t>type</t>
   </si>
@@ -39,169 +39,133 @@
     <t>Hematologic Cancer</t>
   </si>
   <si>
+    <t>0.00 (0.00-0.54)</t>
+  </si>
+  <si>
+    <t>0.00 (0.00-1.98)</t>
+  </si>
+  <si>
+    <t>0.48 (0.21-0.95)</t>
+  </si>
+  <si>
+    <t>0.12 (0.03-0.30)</t>
+  </si>
+  <si>
+    <t>0.68 (0.22-1.58)</t>
+  </si>
+  <si>
+    <t>0.58 (0.38-0.84)</t>
+  </si>
+  <si>
+    <t>0.68 (0.22-1.59)</t>
+  </si>
+  <si>
+    <t>0.75 (0.34-1.41)</t>
+  </si>
+  <si>
+    <t>0.75 (0.62-0.89)</t>
+  </si>
+  <si>
+    <t>Non Melanoma Skin Cancer</t>
+  </si>
+  <si>
+    <t>1.18 (0.51-2.33)</t>
+  </si>
+  <si>
+    <t>1.07 (0.13-3.87)</t>
+  </si>
+  <si>
+    <t>1.14 (0.69-1.78)</t>
+  </si>
+  <si>
+    <t>0.80 (0.53-1.16)</t>
+  </si>
+  <si>
+    <t>0.80 (0.29-1.75)</t>
+  </si>
+  <si>
+    <t>0.85 (0.61-1.16)</t>
+  </si>
+  <si>
+    <t>3.92 (2.62-5.63)</t>
+  </si>
+  <si>
+    <t>3.19 (2.27-4.37)</t>
+  </si>
+  <si>
+    <t>3.12 (2.87-3.40)</t>
+  </si>
+  <si>
+    <t>Solid Cancer</t>
+  </si>
+  <si>
+    <t>1.21 (0.52-2.38)</t>
+  </si>
+  <si>
+    <t>3.95 (1.59-8.13)</t>
+  </si>
+  <si>
+    <t>4.38 (3.41-5.54)</t>
+  </si>
+  <si>
+    <t>1.45 (1.07-1.92)</t>
+  </si>
+  <si>
+    <t>2.93 (1.81-4.48)</t>
+  </si>
+  <si>
+    <t>3.03 (2.55-3.59)</t>
+  </si>
+  <si>
+    <t>5.79 (4.10-7.95)</t>
+  </si>
+  <si>
+    <t>6.82 (5.33-8.60)</t>
+  </si>
+  <si>
+    <t>6.34 (5.95-6.76)</t>
+  </si>
+  <si>
+    <t>Cardiac disease</t>
+  </si>
+  <si>
+    <t>Aortic Insufficiency/Aortic Regurgitation</t>
+  </si>
+  <si>
+    <t>0.60 (0.16-1.53)</t>
+  </si>
+  <si>
+    <t>0.54 (0.01-3.00)</t>
+  </si>
+  <si>
+    <t>1.47 (0.94-2.19)</t>
+  </si>
+  <si>
+    <t>0.66 (0.41-0.99)</t>
+  </si>
+  <si>
+    <t>0.41 (0.08-1.18)</t>
+  </si>
+  <si>
+    <t>0.91 (0.65-1.23)</t>
+  </si>
+  <si>
+    <t>3.47 (2.22-5.16)</t>
+  </si>
+  <si>
+    <t>3.44 (2.45-4.71)</t>
+  </si>
+  <si>
+    <t>3.82 (3.52-4.13)</t>
+  </si>
+  <si>
+    <t>Conduction Block</t>
+  </si>
+  <si>
     <t>0.00 (0.00-0.55)</t>
   </si>
   <si>
-    <t>0.00 (0.00-1.98)</t>
-  </si>
-  <si>
-    <t>0.00 (0.00-1.78)</t>
-  </si>
-  <si>
-    <t>0.56 (0.00-1.10)</t>
-  </si>
-  <si>
-    <t>0.12 (0.03-0.30)</t>
-  </si>
-  <si>
-    <t>0.68 (0.22-1.58)</t>
-  </si>
-  <si>
-    <t>0.50 (0.16-1.17)</t>
-  </si>
-  <si>
-    <t>0.57 (0.03-0.88)</t>
-  </si>
-  <si>
-    <t>0.68 (0.22-1.59)</t>
-  </si>
-  <si>
-    <t>0.75 (0.34-1.41)</t>
-  </si>
-  <si>
-    <t>0.64 (0.34-1.10)</t>
-  </si>
-  <si>
-    <t>0.76 (0.22-0.91)</t>
-  </si>
-  <si>
-    <t>Non Melanoma Skin Cancer</t>
-  </si>
-  <si>
-    <t>1.18 (0.51-2.33)</t>
-  </si>
-  <si>
-    <t>1.07 (0.13-3.88)</t>
-  </si>
-  <si>
-    <t>0.48 (0.01-2.69)</t>
-  </si>
-  <si>
-    <t>1.18 (0.51-1.89)</t>
-  </si>
-  <si>
-    <t>0.80 (0.53-1.16)</t>
-  </si>
-  <si>
-    <t>0.80 (0.29-1.75)</t>
-  </si>
-  <si>
-    <t>0.30 (0.06-0.87)</t>
-  </si>
-  <si>
-    <t>1.00 (0.53-1.39)</t>
-  </si>
-  <si>
-    <t>3.93 (2.63-5.64)</t>
-  </si>
-  <si>
-    <t>3.19 (2.27-4.37)</t>
-  </si>
-  <si>
-    <t>3.91 (3.10-4.86)</t>
-  </si>
-  <si>
-    <t>3.02 (2.63-3.31)</t>
-  </si>
-  <si>
-    <t>Solid Cancer</t>
-  </si>
-  <si>
-    <t>1.21 (0.52-2.39)</t>
-  </si>
-  <si>
-    <t>3.95 (1.59-8.14)</t>
-  </si>
-  <si>
-    <t>1.99 (0.54-5.10)</t>
-  </si>
-  <si>
-    <t>4.80 (0.52-6.11)</t>
-  </si>
-  <si>
-    <t>1.46 (1.07-1.93)</t>
-  </si>
-  <si>
-    <t>2.93 (1.81-4.48)</t>
-  </si>
-  <si>
-    <t>2.17 (1.34-3.32)</t>
-  </si>
-  <si>
-    <t>3.28 (1.07-3.93)</t>
-  </si>
-  <si>
-    <t>5.80 (4.10-7.96)</t>
-  </si>
-  <si>
-    <t>6.81 (5.32-8.59)</t>
-  </si>
-  <si>
-    <t>4.95 (3.96-6.11)</t>
-  </si>
-  <si>
-    <t>6.52 (4.10-6.97)</t>
-  </si>
-  <si>
-    <t>Cardiac disease</t>
-  </si>
-  <si>
-    <t>Aortic Insufficiency/Aortic Regurgitation</t>
-  </si>
-  <si>
-    <t>0.60 (0.16-1.53)</t>
-  </si>
-  <si>
-    <t>0.54 (0.01-3.00)</t>
-  </si>
-  <si>
-    <t>0.98 (0.12-3.55)</t>
-  </si>
-  <si>
-    <t>1.49 (0.16-2.28)</t>
-  </si>
-  <si>
-    <t>0.66 (0.41-1.00)</t>
-  </si>
-  <si>
-    <t>0.41 (0.08-1.18)</t>
-  </si>
-  <si>
-    <t>0.50 (0.16-1.18)</t>
-  </si>
-  <si>
-    <t>1.02 (0.41-1.41)</t>
-  </si>
-  <si>
-    <t>3.48 (2.23-5.18)</t>
-  </si>
-  <si>
-    <t>3.44 (2.45-4.70)</t>
-  </si>
-  <si>
-    <t>3.08 (2.34-3.98)</t>
-  </si>
-  <si>
-    <t>3.93 (2.23-4.27)</t>
-  </si>
-  <si>
-    <t>Conduction Block</t>
-  </si>
-  <si>
-    <t>0.98 (0.12-3.54)</t>
-  </si>
-  <si>
-    <t>0.98 (0.00-1.65)</t>
+    <t>1.03 (0.60-1.65)</t>
   </si>
   <si>
     <t>0.48 (0.27-0.78)</t>
@@ -210,28 +174,22 @@
     <t>0.41 (0.08-1.19)</t>
   </si>
   <si>
-    <t>0.91 (0.41-1.72)</t>
-  </si>
-  <si>
-    <t>1.18 (0.27-1.59)</t>
-  </si>
-  <si>
-    <t>2.75 (1.65-4.29)</t>
+    <t>1.12 (0.84-1.47)</t>
+  </si>
+  <si>
+    <t>2.74 (1.65-4.27)</t>
   </si>
   <si>
     <t>3.55 (2.55-4.82)</t>
   </si>
   <si>
-    <t>2.65 (1.98-3.49)</t>
-  </si>
-  <si>
-    <t>3.16 (1.65-3.46)</t>
+    <t>3.09 (2.83-3.38)</t>
   </si>
   <si>
     <t>Myocardial infarction</t>
   </si>
   <si>
-    <t>0.07 (0.00-0.39)</t>
+    <t>0.06 (0.00-0.33)</t>
   </si>
   <si>
     <t>0.18 (0.07-0.39)</t>
@@ -240,22 +198,16 @@
     <t>0.13 (0.00-0.75)</t>
   </si>
   <si>
-    <t>0.10 (0.00-0.56)</t>
-  </si>
-  <si>
-    <t>0.35 (0.07-0.61)</t>
-  </si>
-  <si>
-    <t>1.37 (0.66-2.52)</t>
+    <t>0.30 (0.16-0.50)</t>
+  </si>
+  <si>
+    <t>1.23 (0.56-2.34)</t>
   </si>
   <si>
     <t>2.03 (1.30-3.03)</t>
   </si>
   <si>
-    <t>1.60 (1.09-2.25)</t>
-  </si>
-  <si>
-    <t>1.17 (0.66-1.36)</t>
+    <t>1.23 (1.07-1.41)</t>
   </si>
   <si>
     <t>Infection</t>
@@ -264,79 +216,61 @@
     <t>Hospitalized infection</t>
   </si>
   <si>
-    <t>2.22 (1.24-3.66)</t>
-  </si>
-  <si>
-    <t>2.15 (0.58-5.50)</t>
-  </si>
-  <si>
-    <t>1.93 (0.53-4.95)</t>
-  </si>
-  <si>
-    <t>3.89 (1.24-5.05)</t>
-  </si>
-  <si>
-    <t>5.16 (4.42-5.99)</t>
+    <t>2.21 (1.24-3.65)</t>
+  </si>
+  <si>
+    <t>2.14 (0.58-5.49)</t>
+  </si>
+  <si>
+    <t>3.60 (2.75-4.63)</t>
+  </si>
+  <si>
+    <t>5.20 (4.46-6.03)</t>
   </si>
   <si>
     <t>4.42 (3.04-6.20)</t>
   </si>
   <si>
-    <t>6.38 (4.91-8.14)</t>
-  </si>
-  <si>
-    <t>5.05 (4.42-5.83)</t>
-  </si>
-  <si>
-    <t>14.48 (11.87-17.50)</t>
-  </si>
-  <si>
-    <t>15.39 (13.27-17.76)</t>
-  </si>
-  <si>
-    <t>19.72 (17.85-21.74)</t>
-  </si>
-  <si>
-    <t>8.70 (11.87-9.18)</t>
+    <t>5.35 (4.70-6.05)</t>
+  </si>
+  <si>
+    <t>14.33 (11.73-17.33)</t>
+  </si>
+  <si>
+    <t>15.40 (13.28-17.76)</t>
+  </si>
+  <si>
+    <t>10.03 (9.57-10.51)</t>
   </si>
   <si>
     <t>Opportunistic infection</t>
   </si>
   <si>
-    <t>1.20 (0.52-2.36)</t>
-  </si>
-  <si>
-    <t>1.63 (0.34-4.77)</t>
-  </si>
-  <si>
-    <t>0.49 (0.01-2.74)</t>
-  </si>
-  <si>
-    <t>0.56 (0.52-1.10)</t>
-  </si>
-  <si>
-    <t>1.26 (0.91-1.71)</t>
+    <t>1.19 (0.52-2.35)</t>
+  </si>
+  <si>
+    <t>1.63 (0.34-4.76)</t>
+  </si>
+  <si>
+    <t>0.54 (0.25-1.03)</t>
+  </si>
+  <si>
+    <t>1.26 (0.91-1.70)</t>
   </si>
   <si>
     <t>1.21 (0.55-2.30)</t>
   </si>
   <si>
-    <t>1.85 (1.10-2.93)</t>
-  </si>
-  <si>
-    <t>1.04 (0.91-1.43)</t>
-  </si>
-  <si>
-    <t>3.07 (1.90-4.69)</t>
-  </si>
-  <si>
-    <t>4.00 (2.90-5.36)</t>
-  </si>
-  <si>
-    <t>3.37 (2.55-4.38)</t>
-  </si>
-  <si>
-    <t>2.08 (1.90-2.32)</t>
+    <t>1.19 (0.89-1.55)</t>
+  </si>
+  <si>
+    <t>3.06 (1.90-4.69)</t>
+  </si>
+  <si>
+    <t>4.00 (2.91-5.37)</t>
+  </si>
+  <si>
+    <t>2.21 (1.98-2.45)</t>
   </si>
   <si>
     <t>Kidney disease</t>
@@ -345,19 +279,16 @@
     <t>Amyloidosis</t>
   </si>
   <si>
-    <t>0.21 (0.00-0.61)</t>
-  </si>
-  <si>
-    <t>0.03 (0.00-0.17)</t>
+    <t>0.18 (0.04-0.53)</t>
+  </si>
+  <si>
+    <t>0.03 (0.00-0.16)</t>
   </si>
   <si>
     <t>0.00 (0.00-0.49)</t>
   </si>
   <si>
-    <t>0.00 (0.00-0.37)</t>
-  </si>
-  <si>
-    <t>0.00 (0.00-0.10)</t>
+    <t>0.00 (0.00-0.08)</t>
   </si>
   <si>
     <t>0.00 (0.00-0.50)</t>
@@ -366,10 +297,7 @@
     <t>0.00 (0.00-0.30)</t>
   </si>
   <si>
-    <t>0.05 (0.00-0.27)</t>
-  </si>
-  <si>
-    <t>0.03 (0.00-0.08)</t>
+    <t>0.03 (0.01-0.07)</t>
   </si>
   <si>
     <t>IgA nephropathy</t>
@@ -378,22 +306,16 @@
     <t>0.30 (0.04-1.08)</t>
   </si>
   <si>
-    <t>0.48 (0.01-2.70)</t>
-  </si>
-  <si>
-    <t>0.00 (0.04-0.26)</t>
-  </si>
-  <si>
     <t>0.09 (0.02-0.26)</t>
   </si>
   <si>
-    <t>0.11 (0.02-0.28)</t>
+    <t>0.09 (0.02-0.22)</t>
   </si>
   <si>
     <t>0.14 (0.00-0.76)</t>
   </si>
   <si>
-    <t>0.06 (0.00-0.11)</t>
+    <t>0.06 (0.03-0.11)</t>
   </si>
   <si>
     <t>Nephrotic syndrome</t>
@@ -402,16 +324,16 @@
     <t>0.30 (0.04-1.07)</t>
   </si>
   <si>
-    <t>0.03 (0.00-0.15)</t>
+    <t>0.00 (0.00-0.22)</t>
+  </si>
+  <si>
+    <t>0.02 (0.00-0.12)</t>
   </si>
   <si>
     <t>0.14 (0.00-0.75)</t>
   </si>
   <si>
-    <t>0.00 (0.00-0.18)</t>
-  </si>
-  <si>
-    <t>0.05 (0.00-0.09)</t>
+    <t>0.04 (0.02-0.08)</t>
   </si>
   <si>
     <t>Lung disease</t>
@@ -429,19 +351,13 @@
     <t>Interstitial lung disease</t>
   </si>
   <si>
-    <t>0.00 (0.00-0.26)</t>
-  </si>
-  <si>
-    <t>0.11 (0.00-0.28)</t>
-  </si>
-  <si>
     <t>0.41 (0.08-1.20)</t>
   </si>
   <si>
     <t>0.50 (0.18-1.09)</t>
   </si>
   <si>
-    <t>0.22 (0.08-0.31)</t>
+    <t>0.20 (0.14-0.28)</t>
   </si>
   <si>
     <t>Restrictive lung disease </t>
@@ -450,13 +366,7 @@
     <t>0.15 (0.00-0.83)</t>
   </si>
   <si>
-    <t>0.00 (0.00-1.99)</t>
-  </si>
-  <si>
-    <t>1.96 (0.53-5.01)</t>
-  </si>
-  <si>
-    <t>0.84 (0.00-1.46)</t>
+    <t>0.97 (0.55-1.57)</t>
   </si>
   <si>
     <t>0.63 (0.39-0.96)</t>
@@ -465,22 +375,16 @@
     <t>0.27 (0.03-0.97)</t>
   </si>
   <si>
-    <t>0.61 (0.22-1.32)</t>
-  </si>
-  <si>
-    <t>1.04 (0.39-1.43)</t>
+    <t>0.95 (0.69-1.27)</t>
   </si>
   <si>
     <t>1.86 (0.99-3.18)</t>
   </si>
   <si>
-    <t>2.57 (1.73-3.66)</t>
-  </si>
-  <si>
-    <t>1.80 (1.25-2.50)</t>
-  </si>
-  <si>
-    <t>1.77 (0.99-1.99)</t>
+    <t>2.57 (1.73-3.67)</t>
+  </si>
+  <si>
+    <t>1.76 (1.57-1.98)</t>
   </si>
   <si>
     <t>Neurological Disease</t>
@@ -489,34 +393,28 @@
     <t>Cauda Equina syndrome</t>
   </si>
   <si>
+    <t>0.04 (0.01-0.15)</t>
+  </si>
+  <si>
     <t>0.08 (0.00-0.46)</t>
   </si>
   <si>
-    <t>0.10 (0.01-0.35)</t>
-  </si>
-  <si>
-    <t>0.04 (0.00-0.08)</t>
+    <t>0.05 (0.02-0.09)</t>
   </si>
   <si>
     <t>Spinal Cord compression</t>
   </si>
   <si>
+    <t>0.12 (0.01-0.43)</t>
+  </si>
+  <si>
     <t>0.15 (0.05-0.35)</t>
   </si>
   <si>
-    <t>0.20 (0.02-0.72)</t>
-  </si>
-  <si>
-    <t>0.05 (0.05-0.20)</t>
-  </si>
-  <si>
     <t>0.25 (0.05-0.72)</t>
   </si>
   <si>
-    <t>0.29 (0.11-0.64)</t>
-  </si>
-  <si>
-    <t>0.14 (0.00-0.21)</t>
+    <t>0.16 (0.10-0.23)</t>
   </si>
   <si>
     <t>Osteoporotic fracture</t>
@@ -531,28 +429,19 @@
     <t>0.54 (0.01-3.01)</t>
   </si>
   <si>
-    <t>1.55 (0.24-2.35)</t>
+    <t>1.40 (0.89-2.10)</t>
   </si>
   <si>
     <t>0.42 (0.23-0.70)</t>
   </si>
   <si>
-    <t>1.00 (0.48-1.85)</t>
-  </si>
-  <si>
-    <t>0.99 (0.23-1.37)</t>
-  </si>
-  <si>
-    <t>2.71 (1.63-4.24)</t>
-  </si>
-  <si>
-    <t>2.00 (1.27-2.99)</t>
-  </si>
-  <si>
-    <t>3.49 (2.70-4.44)</t>
-  </si>
-  <si>
-    <t>2.62 (1.63-2.90)</t>
+    <t>2.71 (1.63-4.23)</t>
+  </si>
+  <si>
+    <t>2.00 (1.27-3.00)</t>
+  </si>
+  <si>
+    <t>2.73 (2.48-2.99)</t>
   </si>
   <si>
     <t>Non-vertebral osteoporotic fracture</t>
@@ -561,37 +450,28 @@
     <t>1.35 (0.62-2.57)</t>
   </si>
   <si>
-    <t>2.19 (0.60-5.61)</t>
-  </si>
-  <si>
-    <t>1.49 (0.31-4.34)</t>
-  </si>
-  <si>
-    <t>1.98 (0.62-2.87)</t>
-  </si>
-  <si>
-    <t>1.05 (0.73-1.47)</t>
+    <t>2.19 (0.60-5.60)</t>
+  </si>
+  <si>
+    <t>1.96 (1.34-2.77)</t>
+  </si>
+  <si>
+    <t>1.08 (0.76-1.50)</t>
   </si>
   <si>
     <t>1.23 (0.56-2.33)</t>
   </si>
   <si>
-    <t>1.42 (0.78-2.39)</t>
-  </si>
-  <si>
-    <t>1.15 (0.73-1.56)</t>
-  </si>
-  <si>
-    <t>4.31 (2.89-6.19)</t>
+    <t>1.21 (0.91-1.57)</t>
+  </si>
+  <si>
+    <t>4.31 (2.88-6.18)</t>
   </si>
   <si>
     <t>3.37 (2.38-4.62)</t>
   </si>
   <si>
-    <t>4.72 (3.77-5.83)</t>
-  </si>
-  <si>
-    <t>3.47 (2.89-3.80)</t>
+    <t>3.62 (3.33-3.92)</t>
   </si>
   <si>
     <t>Disease manifestation</t>
@@ -606,25 +486,19 @@
     <t>1.58 (0.76-2.91)</t>
   </si>
   <si>
-    <t>1.10 (0.13-3.98)</t>
-  </si>
-  <si>
-    <t>0.49 (0.01-2.70)</t>
-  </si>
-  <si>
-    <t>1.35 (0.76-2.10)</t>
-  </si>
-  <si>
-    <t>1.59 (1.18-2.09)</t>
+    <t>1.10 (0.13-3.97)</t>
+  </si>
+  <si>
+    <t>1.22 (0.75-1.89)</t>
+  </si>
+  <si>
+    <t>1.58 (1.18-2.08)</t>
   </si>
   <si>
     <t>1.22 (0.56-2.33)</t>
   </si>
   <si>
-    <t>0.61 (0.22-1.33)</t>
-  </si>
-  <si>
-    <t>2.18 (1.18-2.72)</t>
+    <t>1.84 (1.47-2.28)</t>
   </si>
   <si>
     <t>1.31 (0.60-2.49)</t>
@@ -633,10 +507,7 @@
     <t>0.84 (0.40-1.55)</t>
   </si>
   <si>
-    <t>0.35 (0.14-0.72)</t>
-  </si>
-  <si>
-    <t>0.58 (0.60-0.71)</t>
+    <t>0.55 (0.44-0.67)</t>
   </si>
   <si>
     <t>Ulcerative Colitis</t>
@@ -645,34 +516,25 @@
     <t>0.61 (0.17-1.55)</t>
   </si>
   <si>
-    <t>0.97 (0.12-3.52)</t>
-  </si>
-  <si>
-    <t>1.19 (0.17-1.91)</t>
-  </si>
-  <si>
-    <t>1.41 (1.03-1.88)</t>
+    <t>1.15 (0.69-1.80)</t>
+  </si>
+  <si>
+    <t>1.41 (1.03-1.87)</t>
   </si>
   <si>
     <t>1.91 (1.04-3.20)</t>
   </si>
   <si>
-    <t>0.71 (0.29-1.46)</t>
-  </si>
-  <si>
-    <t>2.00 (1.03-2.52)</t>
-  </si>
-  <si>
-    <t>1.62 (0.81-2.90)</t>
+    <t>1.72 (1.36-2.15)</t>
+  </si>
+  <si>
+    <t>1.62 (0.81-2.89)</t>
   </si>
   <si>
     <t>0.94 (0.47-1.68)</t>
   </si>
   <si>
-    <t>0.70 (0.38-1.17)</t>
-  </si>
-  <si>
-    <t>0.77 (0.81-0.92)</t>
+    <t>0.76 (0.64-0.90)</t>
   </si>
   <si>
     <t>PsO/PsA</t>
@@ -681,28 +543,22 @@
     <t>Psoriasis</t>
   </si>
   <si>
-    <t>1.45 (0.66-2.75)</t>
-  </si>
-  <si>
-    <t>0.00 (0.00-2.09)</t>
-  </si>
-  <si>
-    <t>1.02 (0.12-3.67)</t>
-  </si>
-  <si>
-    <t>1.29 (0.66-2.04)</t>
-  </si>
-  <si>
-    <t>2.10 (1.62-2.67)</t>
+    <t>1.44 (0.66-2.74)</t>
+  </si>
+  <si>
+    <t>0.00 (0.00-2.08)</t>
+  </si>
+  <si>
+    <t>1.24 (0.76-1.92)</t>
+  </si>
+  <si>
+    <t>2.09 (1.61-2.66)</t>
   </si>
   <si>
     <t>1.73 (0.90-3.03)</t>
   </si>
   <si>
-    <t>1.36 (0.72-2.32)</t>
-  </si>
-  <si>
-    <t>1.28 (1.62-1.71)</t>
+    <t>1.32 (1.00-1.69)</t>
   </si>
   <si>
     <t>2.37 (1.33-3.91)</t>
@@ -711,10 +567,7 @@
     <t>0.81 (0.37-1.54)</t>
   </si>
   <si>
-    <t>0.82 (0.47-1.34)</t>
-  </si>
-  <si>
-    <t>1.17 (1.33-1.35)</t>
+    <t>1.13 (0.97-1.30)</t>
   </si>
   <si>
     <t>Psoriatic arthritis</t>
@@ -723,76 +576,58 @@
     <t>2.10 (1.12-3.59)</t>
   </si>
   <si>
-    <t>1.73 (0.36-5.04)</t>
-  </si>
-  <si>
-    <t>1.52 (0.31-4.44)</t>
-  </si>
-  <si>
-    <t>1.52 (1.12-2.32)</t>
-  </si>
-  <si>
-    <t>2.81 (2.24-3.46)</t>
+    <t>1.72 (0.36-5.04)</t>
+  </si>
+  <si>
+    <t>1.50 (0.96-2.23)</t>
+  </si>
+  <si>
+    <t>2.79 (2.24-3.45)</t>
   </si>
   <si>
     <t>4.25 (2.85-6.11)</t>
   </si>
   <si>
-    <t>0.52 (0.17-1.21)</t>
-  </si>
-  <si>
-    <t>1.73 (2.24-2.22)</t>
-  </si>
-  <si>
-    <t>2.63 (1.53-4.21)</t>
+    <t>1.49 (1.16-1.89)</t>
+  </si>
+  <si>
+    <t>2.62 (1.53-4.20)</t>
   </si>
   <si>
     <t>1.73 (1.04-2.70)</t>
   </si>
   <si>
-    <t>0.87 (0.51-1.40)</t>
-  </si>
-  <si>
-    <t>0.47 (1.53-0.59)</t>
+    <t>0.52 (0.42-0.64)</t>
   </si>
   <si>
     <t>Uveitis</t>
   </si>
   <si>
-    <t>3.09 (1.86-4.82)</t>
-  </si>
-  <si>
-    <t>3.39 (1.24-7.38)</t>
-  </si>
-  <si>
-    <t>2.00 (0.55-5.12)</t>
-  </si>
-  <si>
-    <t>2.99 (1.86-4.06)</t>
-  </si>
-  <si>
-    <t>3.45 (2.83-4.18)</t>
+    <t>3.08 (1.86-4.82)</t>
+  </si>
+  <si>
+    <t>3.39 (1.24-7.37)</t>
+  </si>
+  <si>
+    <t>2.83 (2.07-3.79)</t>
+  </si>
+  <si>
+    <t>3.44 (2.82-4.16)</t>
   </si>
   <si>
     <t>2.83 (1.73-4.37)</t>
   </si>
   <si>
-    <t>2.83 (1.87-4.12)</t>
-  </si>
-  <si>
-    <t>3.63 (2.83-4.32)</t>
-  </si>
-  <si>
-    <t>2.31 (1.32-3.76)</t>
+    <t>3.48 (2.95-4.07)</t>
+  </si>
+  <si>
+    <t>2.31 (1.32-3.75)</t>
   </si>
   <si>
     <t>1.46 (0.85-2.34)</t>
   </si>
   <si>
-    <t>0.85 (0.49-1.36)</t>
-  </si>
-  <si>
-    <t>0.55 (1.32-0.69)</t>
+    <t>0.59 (0.48-0.71)</t>
   </si>
   <si>
     <t>MPCD
@@ -804,11 +639,7 @@
   </si>
   <si>
     <t>MPCD
-NSAID</t>
-  </si>
-  <si>
-    <t>MPCD
-No exposure</t>
+NSAID or no exposure</t>
   </si>
   <si>
     <t>Marketscan
@@ -820,11 +651,7 @@
   </si>
   <si>
     <t>Marketscan
-NSAID</t>
-  </si>
-  <si>
-    <t>Marketscan
-No exposure</t>
+NSAID or no exposure</t>
   </si>
   <si>
     <t>Medicare
@@ -836,11 +663,7 @@
   </si>
   <si>
     <t>Medicare
-NSAID</t>
-  </si>
-  <si>
-    <t>Medicare
-No exposure</t>
+NSAID or no exposure</t>
   </si>
 </sst>
 </file>
@@ -1377,16 +1200,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1428,24 +1242,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O24" totalsRowShown="0">
-  <autoFilter ref="A1:O24"/>
-  <tableColumns count="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:L24" totalsRowShown="0">
+  <autoFilter ref="A1:L24"/>
+  <tableColumns count="12">
     <tableColumn id="1" name="type"/>
     <tableColumn id="2" name="outcomeCategory"/>
     <tableColumn id="3" name="disease"/>
-    <tableColumn id="4" name="MPCD_x000a_TNF" dataDxfId="11"/>
-    <tableColumn id="5" name="MPCD_x000a_DMARD" dataDxfId="10"/>
-    <tableColumn id="6" name="MPCD_x000a_NSAID" dataDxfId="9"/>
-    <tableColumn id="7" name="MPCD_x000a_No exposure" dataDxfId="8"/>
-    <tableColumn id="8" name="Marketscan_x000a_TNF" dataDxfId="7"/>
-    <tableColumn id="9" name="Marketscan_x000a_DMARD" dataDxfId="6"/>
-    <tableColumn id="10" name="Marketscan_x000a_NSAID" dataDxfId="5"/>
-    <tableColumn id="11" name="Marketscan_x000a_No exposure" dataDxfId="4"/>
-    <tableColumn id="12" name="Medicare_x000a_TNF" dataDxfId="3"/>
-    <tableColumn id="13" name="Medicare_x000a_DMARD" dataDxfId="2"/>
-    <tableColumn id="14" name="Medicare_x000a_NSAID" dataDxfId="1"/>
-    <tableColumn id="15" name="Medicare_x000a_No exposure" dataDxfId="0"/>
+    <tableColumn id="4" name="MPCD_x000a_TNF" dataDxfId="8"/>
+    <tableColumn id="5" name="MPCD_x000a_DMARD" dataDxfId="7"/>
+    <tableColumn id="6" name="MPCD_x000a_NSAID or no exposure" dataDxfId="6"/>
+    <tableColumn id="7" name="Marketscan_x000a_TNF" dataDxfId="5"/>
+    <tableColumn id="8" name="Marketscan_x000a_DMARD" dataDxfId="4"/>
+    <tableColumn id="9" name="Marketscan_x000a_NSAID or no exposure" dataDxfId="3"/>
+    <tableColumn id="10" name="Medicare_x000a_TNF" dataDxfId="2"/>
+    <tableColumn id="11" name="Medicare_x000a_DMARD" dataDxfId="1"/>
+    <tableColumn id="12" name="Medicare_x000a_NSAID or no exposure" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1714,7 +1525,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1723,15 +1534,15 @@
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1742,43 +1553,34 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>258</v>
+        <v>203</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>259</v>
+        <v>204</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>260</v>
+        <v>205</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>261</v>
+        <v>206</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>262</v>
+        <v>207</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>263</v>
+        <v>208</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>264</v>
+        <v>209</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>265</v>
+        <v>210</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>269</v>
+        <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1815,17 +1617,8 @@
       <c r="L2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1833,46 +1626,37 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1880,148 +1664,121 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>43</v>
-      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C5" t="s">
+      <c r="L5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -2030,139 +1787,112 @@
         <v>7</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="I9" s="2" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
@@ -2171,139 +1901,112 @@
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>119</v>
+        <v>56</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>127</v>
+        <v>91</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
@@ -2312,45 +2015,36 @@
         <v>7</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>133</v>
+        <v>88</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
@@ -2359,92 +2053,74 @@
         <v>7</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="I14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="L14" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="C15" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>143</v>
+        <v>7</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>153</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>154</v>
+        <v>122</v>
       </c>
       <c r="C16" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>6</v>
@@ -2453,45 +2129,36 @@
         <v>7</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>6</v>
@@ -2500,363 +2167,291 @@
         <v>7</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>160</v>
+        <v>88</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>161</v>
+        <v>103</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>162</v>
+        <v>130</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="C18" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>170</v>
+        <v>137</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>171</v>
+        <v>117</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
       <c r="B19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>151</v>
+      </c>
+      <c r="B20" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B21" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21" t="s">
+        <v>163</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C19" t="s">
+      <c r="H21" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>151</v>
+      </c>
+      <c r="B22" t="s">
+        <v>172</v>
+      </c>
+      <c r="C22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="K22" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="L22" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="H19" s="2" t="s">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" t="s">
         <v>183</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="N19" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="O19" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>190</v>
       </c>
+      <c r="K23" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>192</v>
+      </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>191</v>
-      </c>
-      <c r="B20" t="s">
-        <v>192</v>
-      </c>
-      <c r="C20" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>151</v>
+      </c>
+      <c r="B24" t="s">
         <v>193</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="C24" t="s">
+        <v>193</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="K24" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="L24" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>191</v>
-      </c>
-      <c r="B21" t="s">
-        <v>192</v>
-      </c>
-      <c r="C21" t="s">
-        <v>206</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>191</v>
-      </c>
-      <c r="B22" t="s">
-        <v>218</v>
-      </c>
-      <c r="C22" t="s">
-        <v>219</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>191</v>
-      </c>
-      <c r="B23" t="s">
-        <v>218</v>
-      </c>
-      <c r="C23" t="s">
-        <v>232</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>191</v>
-      </c>
-      <c r="B24" t="s">
-        <v>245</v>
-      </c>
-      <c r="C24" t="s">
-        <v>245</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="O24" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>